<commit_message>
Added all the transition values and Updated code
</commit_message>
<xml_diff>
--- a/Fuzzy Transition Calculation.xlsx
+++ b/Fuzzy Transition Calculation.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC0CF31C-260A-42A6-96D6-C662B1936EDE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F95832F-48A2-4BF1-BB72-8127CD1E8E91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>SYMBOL</t>
   </si>
@@ -50,17 +55,44 @@
     <t xml:space="preserve">Natural </t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Flat</t>
+  </si>
+  <si>
+    <t>Accent</t>
+  </si>
+  <si>
+    <t>Crochet</t>
+  </si>
+  <si>
+    <t>8th Rest</t>
+  </si>
+  <si>
+    <t>Quarter Rest</t>
+  </si>
+  <si>
+    <t>Quaver</t>
+  </si>
+  <si>
+    <t>16th Rest</t>
+  </si>
+  <si>
+    <t>Slur</t>
+  </si>
+  <si>
+    <t>Staccatissimo</t>
+  </si>
+  <si>
+    <t>32nd Rest</t>
+  </si>
+  <si>
+    <t>Minim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,13 +132,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -425,23 +457,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -457,145 +489,420 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>-14</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="1">
+        <v>-12</v>
+      </c>
+      <c r="C3" s="1">
         <v>-5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-15</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2">
+      <c r="B4" s="1">
+        <v>-21</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-18</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-26</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-22</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-30</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-18</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-34</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-29</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-18</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-27</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-10</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-16</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-16</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-60</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>81</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>21</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-13</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-18</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-18</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-17</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>21</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-15</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-21</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1">
+        <v>25</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2">
-        <v>-13</v>
-      </c>
-      <c r="G3" s="2">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>-23</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-8</v>
-      </c>
-      <c r="D4" s="2">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2">
-        <v>-18</v>
-      </c>
-      <c r="G4" s="2">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>-17</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-10</v>
-      </c>
-      <c r="D5" s="2">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="G5" s="2">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
+      <c r="B18" s="1">
+        <v>-41</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-7</v>
+      </c>
+      <c r="D18" s="1">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
-        <v>-12</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-8</v>
-      </c>
-      <c r="D6" s="2">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2">
-        <v>-10</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>-13</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E18" s="1">
+        <v>44</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-24</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -604,5 +911,6 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>